<commit_message>
update 202007022 20:30 a. 优化批量执行SQL b. 新增String类型转String[]方法
</commit_message>
<xml_diff>
--- a/src/main/resource/testCase1data.xlsx
+++ b/src/main/resource/testCase1data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19815" windowHeight="9420"/>
+    <workbookView windowWidth="27195" windowHeight="14100"/>
   </bookViews>
   <sheets>
     <sheet name="init" sheetId="7" r:id="rId1"/>
@@ -54,7 +54,7 @@
     <t xml:space="preserve">Init SQL </t>
   </si>
   <si>
-    <t>"UPDATE `user`  SET `name` = '444' WHERE login_name LIKE '1990000000%' AND `name` = '111';","UPDATE `user`  SET `name` = '333' WHERE login_name LIKE '1990000000%' AND `name` = '222';"</t>
+    <t>UPDATE `user`  SET `name` = '444' WHERE login_name LIKE '1990000000%' AND `name` = '222';,UPDATE `user`  SET `name` = '333' WHERE login_name LIKE '1990000000%' AND `name` = '666';</t>
   </si>
   <si>
     <t>UPDATE `user`  SET `name` = '444' WHERE login_name LIKE '1990000000%' AND `name` = '222';,UPDATE `user`  SET `name` = '333' WHERE login_name LIKE '1990000000%' AND `name` = '111';</t>
@@ -1721,10 +1721,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -1754,6 +1754,29 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1797,47 +1820,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1865,19 +1860,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1917,6 +1917,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1930,6 +1960,54 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1984,84 +2062,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2126,21 +2126,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -2161,26 +2146,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2217,6 +2182,41 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -2231,10 +2231,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2243,133 +2243,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2722,7 +2722,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.25" outlineLevelRow="1" outlineLevelCol="7"/>
@@ -2738,7 +2738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" s="3" customFormat="1" ht="51.75" spans="1:8">
+    <row r="2" s="3" customFormat="1" ht="72" customHeight="1" spans="1:8">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>

</xml_diff>